<commit_message>
added cash requests statistics
</commit_message>
<xml_diff>
--- a/project_dataset/Lexique - Data Analyst.xlsx
+++ b/project_dataset/Lexique - Data Analyst.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd4a035e5905c4ac/Desktop/Ironhack/week_3/project/project-ironhack-payments-en/project_dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB15CBAF-2576-B54A-B443-C252914C6EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{DB15CBAF-2576-B54A-B443-C252914C6EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B4E7B29-2306-432D-A4B0-304A23AE5EAB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="context - fees" sheetId="2" r:id="rId1"/>
@@ -1013,7 +1013,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1199,6 +1199,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1360,13 +1366,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1724,8 +1731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B1B98DC-AA23-8848-AD79-7CDAFD86BA20}">
   <dimension ref="A1:B16376"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -81805,8 +81812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5D6A73B-D1D2-0341-9B4F-0C7C22352858}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -81896,10 +81903,10 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>